<commit_message>
Update BBDD Consolidada (version 1).xlsb.xlsx
Arreglos
</commit_message>
<xml_diff>
--- a/BBDD Consolidada (version 1).xlsb.xlsx
+++ b/BBDD Consolidada (version 1).xlsb.xlsx
@@ -5,17 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fcoyo\Desktop\Tesis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fcoyo\Documents\GitHub\Tesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0EC3B06-D7B5-4202-BE01-D5951AED52A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{938696DA-D6CA-404C-8546-A6686B3592BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1455" yWindow="615" windowWidth="14400" windowHeight="8685" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4665" yWindow="570" windowWidth="14400" windowHeight="8685" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DATOS_NOMBRESLARGOS" sheetId="1" r:id="rId1"/>
     <sheet name="DATOS" sheetId="2" r:id="rId2"/>
     <sheet name="DATOS.TS" sheetId="3" r:id="rId3"/>
+    <sheet name="Estadistica Descriptiva" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
 </workbook>
@@ -986,7 +987,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="34">
   <si>
     <t>Periodo</t>
   </si>
@@ -1056,15 +1057,49 @@
   <si>
     <t>crisis_económica</t>
   </si>
+  <si>
+    <t>Causalidad de Granger</t>
+  </si>
+  <si>
+    <t>desde:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hacia: </t>
+  </si>
+  <si>
+    <t>Tipo de Cambio Real</t>
+  </si>
+  <si>
+    <t>Precio del Cobre</t>
+  </si>
+  <si>
+    <t>Orden</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p-value </t>
+  </si>
+  <si>
+    <t>Presencia de Causalidad</t>
+  </si>
+  <si>
+    <t>TPM</t>
+  </si>
+  <si>
+    <t>IPC</t>
+  </si>
+  <si>
+    <t>Doble Causalidad</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="mmm\.yyyy"/>
+    <numFmt numFmtId="165" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1135,8 +1170,14 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1167,8 +1208,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -1211,11 +1264,146 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1271,6 +1459,45 @@
     </xf>
     <xf numFmtId="3" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -49165,7 +49392,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC272FD2-5EC4-4BE4-878F-346441666433}">
   <dimension ref="A1:J145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A92" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+    <sheetView zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
       <selection activeCell="J97" sqref="J97"/>
     </sheetView>
   </sheetViews>
@@ -53824,10 +54051,314 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35EA5142-E3F9-4F44-9674-B41C6DD2952D}">
+  <dimension ref="B1:G15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="3" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" customWidth="1"/>
+    <col min="6" max="6" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="28"/>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="34" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="35">
+        <v>7.2379999999999996E-3</v>
+      </c>
+      <c r="E4" s="36">
+        <v>1</v>
+      </c>
+      <c r="F4" s="36" t="str">
+        <f>IF(D4&lt;0.05, "Sí","No")</f>
+        <v>Sí</v>
+      </c>
+      <c r="G4" s="37" t="str">
+        <f>IF(AND(F4=F5, F4="Sí"), "Sí", "No")</f>
+        <v>Sí</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="35">
+        <v>1.6809999999999999E-2</v>
+      </c>
+      <c r="E5" s="36">
+        <v>1</v>
+      </c>
+      <c r="F5" s="36" t="str">
+        <f t="shared" ref="F5:F18" si="0">IF(D5&lt;0.05, "Sí","No")</f>
+        <v>Sí</v>
+      </c>
+      <c r="G5" s="37"/>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="35">
+        <v>0.1205</v>
+      </c>
+      <c r="E6" s="36">
+        <v>12</v>
+      </c>
+      <c r="F6" s="36" t="str">
+        <f t="shared" si="0"/>
+        <v>No</v>
+      </c>
+      <c r="G6" s="37" t="str">
+        <f t="shared" ref="G5:G17" si="1">IF(AND(F6=F7, F6="Sí"), "Sí", "No")</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="35">
+        <v>2.614E-2</v>
+      </c>
+      <c r="E7" s="36">
+        <v>3</v>
+      </c>
+      <c r="F7" s="36" t="str">
+        <f t="shared" si="0"/>
+        <v>Sí</v>
+      </c>
+      <c r="G7" s="37"/>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="35">
+        <v>0.64249999999999996</v>
+      </c>
+      <c r="E8" s="36">
+        <v>12</v>
+      </c>
+      <c r="F8" s="36" t="str">
+        <f t="shared" si="0"/>
+        <v>No</v>
+      </c>
+      <c r="G8" s="37" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="35">
+        <v>2.7589999999999998E-4</v>
+      </c>
+      <c r="E9" s="36">
+        <v>1</v>
+      </c>
+      <c r="F9" s="36" t="str">
+        <f t="shared" si="0"/>
+        <v>Sí</v>
+      </c>
+      <c r="G9" s="37"/>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="35">
+        <v>2.035E-2</v>
+      </c>
+      <c r="E10" s="36">
+        <v>1</v>
+      </c>
+      <c r="F10" s="36" t="str">
+        <f t="shared" si="0"/>
+        <v>Sí</v>
+      </c>
+      <c r="G10" s="37" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="35">
+        <v>0.28920000000000001</v>
+      </c>
+      <c r="E11" s="36">
+        <v>12</v>
+      </c>
+      <c r="F11" s="36" t="str">
+        <f t="shared" si="0"/>
+        <v>No</v>
+      </c>
+      <c r="G11" s="37"/>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="35">
+        <v>2.833E-3</v>
+      </c>
+      <c r="E12" s="36">
+        <v>1</v>
+      </c>
+      <c r="F12" s="36" t="str">
+        <f t="shared" si="0"/>
+        <v>Sí</v>
+      </c>
+      <c r="G12" s="37" t="str">
+        <f t="shared" si="1"/>
+        <v>Sí</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="35">
+        <v>2.3699999999999999E-2</v>
+      </c>
+      <c r="E13" s="36">
+        <v>1</v>
+      </c>
+      <c r="F13" s="36" t="str">
+        <f t="shared" si="0"/>
+        <v>Sí</v>
+      </c>
+      <c r="G13" s="37"/>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="35">
+        <v>0.1792</v>
+      </c>
+      <c r="E14" s="36">
+        <v>12</v>
+      </c>
+      <c r="F14" s="36" t="str">
+        <f t="shared" si="0"/>
+        <v>No</v>
+      </c>
+      <c r="G14" s="37" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="38">
+        <v>0.64670000000000005</v>
+      </c>
+      <c r="E15" s="39">
+        <v>12</v>
+      </c>
+      <c r="F15" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>No</v>
+      </c>
+      <c r="G15" s="40"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:G2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -53995,19 +54526,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AD324055-1338-4DF6-8FEE-42FB9AAA38D7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3DD32C1C-3DB8-4C8D-B863-300A0DFAA3C5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -54031,9 +54558,10 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3DD32C1C-3DB8-4C8D-B863-300A0DFAA3C5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AD324055-1338-4DF6-8FEE-42FB9AAA38D7}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>